<commit_message>
Renamed Thermdat to Nasa. Changed excel import function. Bug fixes.
</commit_message>
<xml_diff>
--- a/examples/VASP_to_thermdat/references.xlsx
+++ b/examples/VASP_to_thermdat/references.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UDel Documents\UDel Research\Thermochemistry\Thermochemistry\examples\VASP_to_thermdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3B2903-DD75-4935-9D21-60F0ACAC3EDE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -113,12 +114,6 @@
     <t>elements~O</t>
   </si>
   <si>
-    <t>Type of thermodynamic model. Supported ones can be found in Thermochemistry.models.statmech</t>
-  </si>
-  <si>
-    <t>Thermochemistry.models.statmech.idealgasthermo.IdealGasThermo</t>
-  </si>
-  <si>
     <t>vib_wavenumber~1</t>
   </si>
   <si>
@@ -129,12 +124,18 @@
   </si>
   <si>
     <t>Vibrational wavenumber in 1/cm</t>
+  </si>
+  <si>
+    <t>IdealGas</t>
+  </si>
+  <si>
+    <t>Type of thermodynamic model. Supported models include IdealGas and Harmonic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,31 +499,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,20 +561,20 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -585,7 +586,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>17</v>
@@ -609,20 +610,20 @@
         <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -636,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>298</v>
@@ -663,7 +664,7 @@
         <v>4306.1792999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -677,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>298</v>
@@ -711,16 +712,16 @@
         <v>1582.432</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>

</xml_diff>

<commit_message>
Updated README. Changed excel importing to take relative references.
</commit_message>
<xml_diff>
--- a/examples/VASP_to_thermdat/references.xlsx
+++ b/examples/VASP_to_thermdat/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UDel Documents\UDel Research\Thermochemistry\Thermochemistry\examples\VASP_to_thermdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3B2903-DD75-4935-9D21-60F0ACAC3EDE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EC1FE1-C935-446A-AC9B-F4FA87550F5B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,12 +102,6 @@
     <t>Stoichiometric formula</t>
   </si>
   <si>
-    <t>G:\My Drive\UDel Documents\UDel Research\Thermochemistry\Thermochemistry\examples\VASP_to_thermdat\H2\CONTCAR</t>
-  </si>
-  <si>
-    <t>G:\My Drive\UDel Documents\UDel Research\Thermochemistry\Thermochemistry\examples\VASP_to_thermdat\H2O\CONTCAR</t>
-  </si>
-  <si>
     <t>elements~H</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>Type of thermodynamic model. Supported models include IdealGas and Harmonic</t>
+  </si>
+  <si>
+    <t>.\H2\CONTCAR</t>
+  </si>
+  <si>
+    <t>.\H2O\CONTCAR</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,10 +531,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -561,13 +561,13 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -586,7 +586,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>17</v>
@@ -610,13 +610,13 @@
         <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -637,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>298</v>
@@ -652,7 +652,7 @@
         <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>298</v>
@@ -694,7 +694,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K4">
         <v>2</v>

</xml_diff>